<commit_message>
Lab 3 finalized commit
</commit_message>
<xml_diff>
--- a/assignments/Lab3_Tables.xlsx
+++ b/assignments/Lab3_Tables.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18165\Documents\R\Lab\biostatlab\assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C80103E-63DD-4C91-BCD0-8A2720274E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFDD9F13-04E7-4B79-879D-E55AE3D43D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{BFF9CCF7-7857-41CB-8234-CF6D12DA6E19}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{BFF9CCF7-7857-41CB-8234-CF6D12DA6E19}"/>
   </bookViews>
   <sheets>
-    <sheet name="Table 1 = Cont. Summary Stats" sheetId="5" r:id="rId1"/>
+    <sheet name="Table 1 - Cont. Summary Stats" sheetId="5" r:id="rId1"/>
     <sheet name="Table 2 - Cat. Freq. Counts" sheetId="2" r:id="rId2"/>
     <sheet name="Table 3 - Cat. M of Assoc." sheetId="3" r:id="rId3"/>
   </sheets>
@@ -437,9 +437,6 @@
 p-value</t>
   </si>
   <si>
-    <t>All Subjects</t>
-  </si>
-  <si>
     <t>Dead</t>
   </si>
   <si>
@@ -581,6 +578,9 @@
   </si>
   <si>
     <t xml:space="preserve">How to use Lab 3 tables: </t>
+  </si>
+  <si>
+    <t>All Children</t>
   </si>
 </sst>
 </file>
@@ -959,34 +959,61 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1005,33 +1032,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
@@ -1384,92 +1384,92 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="33"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+    </row>
+    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-    </row>
-    <row r="9" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" s="31" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="32"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-    </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>59</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
@@ -1482,9 +1482,9 @@
       <c r="K12" s="15"/>
     </row>
     <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="37"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -1493,13 +1493,13 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="36"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
     </row>
     <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="37"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -1508,13 +1508,13 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
     </row>
     <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="38"/>
+      <c r="A15" s="36"/>
       <c r="B15" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="15"/>
@@ -1527,11 +1527,11 @@
       <c r="K15" s="15"/>
     </row>
     <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="29" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -1544,9 +1544,9 @@
       <c r="K16" s="17"/>
     </row>
     <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="34"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -1555,13 +1555,13 @@
       <c r="G17" s="16"/>
       <c r="H17" s="16"/>
       <c r="I17" s="16"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="33"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
     </row>
     <row r="18" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="34"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -1570,11 +1570,11 @@
       <c r="G18" s="16"/>
       <c r="H18" s="16"/>
       <c r="I18" s="16"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
     </row>
     <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="35"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="16" t="s">
         <v>12</v>
       </c>
@@ -1590,20 +1590,11 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="K13:K14"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="A9:K9"/>
     <mergeCell ref="A10:A11"/>
@@ -1614,6 +1605,15 @@
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="H10:H11"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K13:K14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -1624,8 +1624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13CF663A-15E9-4E7D-8832-0D087C34448F}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1636,60 +1636,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="30" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="51"/>
+      <c r="E3" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="51"/>
+      <c r="G3" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="51"/>
+      <c r="I3" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="42"/>
-      <c r="E3" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="42"/>
-      <c r="G3" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="42"/>
-      <c r="I3" s="39" t="s">
+      <c r="J3" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="39" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="32"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
@@ -1698,29 +1698,29 @@
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="45" t="s">
-        <v>18</v>
+      <c r="A6" s="39" t="s">
+        <v>17</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1728,13 +1728,13 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
     </row>
     <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="53"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1742,11 +1742,11 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="46"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
@@ -1760,11 +1760,11 @@
       <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="47" t="s">
-        <v>54</v>
+      <c r="A9" s="41" t="s">
+        <v>53</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -1772,13 +1772,13 @@
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="48"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -1786,11 +1786,11 @@
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
     </row>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="49"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="7" t="s">
         <v>12</v>
       </c>
@@ -1804,11 +1804,11 @@
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="50" t="s">
+      <c r="A12" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>22</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>23</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -1816,13 +1816,13 @@
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="50"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
     </row>
     <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="51"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -1830,11 +1830,11 @@
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="52"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
     </row>
     <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="52"/>
+      <c r="A14" s="46"/>
       <c r="B14" s="11" t="s">
         <v>12</v>
       </c>
@@ -1848,11 +1848,11 @@
       <c r="J14" s="12"/>
     </row>
     <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>25</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>26</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -1860,13 +1860,13 @@
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="36"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
     </row>
     <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="37"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
@@ -1874,13 +1874,13 @@
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="37"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
@@ -1888,11 +1888,11 @@
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="38"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="13" t="s">
         <v>12</v>
       </c>
@@ -1906,11 +1906,11 @@
       <c r="J18" s="15"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="16" t="s">
         <v>29</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>30</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
@@ -1918,13 +1918,13 @@
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
       <c r="H19" s="16"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
     </row>
     <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="34"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
@@ -1932,13 +1932,13 @@
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="34"/>
+      <c r="A21" s="30"/>
       <c r="B21" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -1946,11 +1946,11 @@
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
       <c r="H21" s="16"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
     </row>
     <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="35"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="16" t="s">
         <v>12</v>
       </c>
@@ -1965,11 +1965,23 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:D4"/>
+    <mergeCell ref="E3:F4"/>
+    <mergeCell ref="G3:H4"/>
     <mergeCell ref="A19:A22"/>
     <mergeCell ref="I19:I21"/>
     <mergeCell ref="J19:J21"/>
@@ -1982,18 +1994,6 @@
     <mergeCell ref="I12:I13"/>
     <mergeCell ref="J12:J13"/>
     <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:D4"/>
-    <mergeCell ref="E3:F4"/>
-    <mergeCell ref="G3:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2005,7 +2005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EABD559-3FF4-453B-8964-3117EECF2A87}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
@@ -2017,17 +2017,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="A1" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="54"/>
       <c r="C2" s="55"/>
@@ -2046,13 +2046,13 @@
       <c r="A3" s="20"/>
       <c r="B3" s="22"/>
       <c r="C3" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="25" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F3" s="27"/>
       <c r="G3" s="28"/>
@@ -2075,33 +2075,33 @@
         <v>2</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="21" t="s">
         <v>43</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>44</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -2115,9 +2115,9 @@
       <c r="L5" s="12"/>
     </row>
     <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="53"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2131,7 +2131,7 @@
       <c r="L6" s="5"/>
     </row>
     <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="46"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
@@ -2147,11 +2147,11 @@
       <c r="L7" s="17"/>
     </row>
     <row r="8" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="47" t="s">
-        <v>54</v>
+      <c r="A8" s="41" t="s">
+        <v>53</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -2165,9 +2165,9 @@
       <c r="L8" s="12"/>
     </row>
     <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="48"/>
+      <c r="A9" s="42"/>
       <c r="B9" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -2181,7 +2181,7 @@
       <c r="L9" s="7"/>
     </row>
     <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="49"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="7" t="s">
         <v>12</v>
       </c>
@@ -2197,11 +2197,11 @@
       <c r="L10" s="17"/>
     </row>
     <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="50" t="s">
-        <v>22</v>
+      <c r="A11" s="44" t="s">
+        <v>21</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -2215,9 +2215,9 @@
       <c r="L11" s="12"/>
     </row>
     <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="51"/>
+      <c r="A12" s="45"/>
       <c r="B12" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -2231,7 +2231,7 @@
       <c r="L12" s="11"/>
     </row>
     <row r="13" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="52"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="11" t="s">
         <v>12</v>
       </c>
@@ -2247,11 +2247,11 @@
       <c r="L13" s="17"/>
     </row>
     <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>47</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>48</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -2265,9 +2265,9 @@
       <c r="L14" s="12"/>
     </row>
     <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="37"/>
+      <c r="A15" s="35"/>
       <c r="B15" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
@@ -2281,9 +2281,9 @@
       <c r="L15" s="13"/>
     </row>
     <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="37"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
@@ -2297,7 +2297,7 @@
       <c r="L16" s="13"/>
     </row>
     <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="38"/>
+      <c r="A17" s="36"/>
       <c r="B17" s="13" t="s">
         <v>12</v>
       </c>
@@ -2313,11 +2313,11 @@
       <c r="L17" s="17"/>
     </row>
     <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="33" t="s">
-        <v>29</v>
+      <c r="A18" s="29" t="s">
+        <v>28</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
@@ -2331,9 +2331,9 @@
       <c r="L18" s="12"/>
     </row>
     <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="34"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
@@ -2347,9 +2347,9 @@
       <c r="L19" s="16"/>
     </row>
     <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="34"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
@@ -2363,7 +2363,7 @@
       <c r="L20" s="16"/>
     </row>
     <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="35"/>
+      <c r="A21" s="31"/>
       <c r="B21" s="16" t="s">
         <v>12</v>
       </c>
@@ -2380,7 +2380,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>